<commit_message>
Added new team tasks
</commit_message>
<xml_diff>
--- a/Tasks/Tasks.xlsx
+++ b/Tasks/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="12495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>№</t>
   </si>
@@ -133,6 +133,27 @@
   </si>
   <si>
     <t>1. team review 2. all figures are uploaded in github in editable format in design folder 3. all figures are uploaded in document folder as jpg 4. present to a team</t>
+  </si>
+  <si>
+    <t>Task 5 is finished</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Filled historicaldata (solutions and tickets) in SupportTicketingSystem/BackendSystem/HISTORYDATA.xlsx</t>
+  </si>
+  <si>
+    <t>1. team review</t>
+  </si>
+  <si>
+    <t>Tasks 1-11 are finished</t>
+  </si>
+  <si>
+    <t>Tasks 1-12 are finished</t>
+  </si>
+  <si>
+    <t>Check ODATA API with POSTMAN. Do we have all ODATA functionality regarding our mockup?</t>
   </si>
 </sst>
 </file>
@@ -480,21 +501,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -514,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -534,7 +555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -554,7 +575,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -574,7 +595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -594,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -614,7 +635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -634,7 +655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -654,7 +675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -671,7 +692,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -691,7 +712,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -708,7 +729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -723,6 +744,106 @@
       </c>
       <c r="E12" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added task for Ilkay 8b
</commit_message>
<xml_diff>
--- a/Tasks/Tasks.xlsx
+++ b/Tasks/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>№</t>
   </si>
@@ -163,6 +163,24 @@
   </si>
   <si>
     <t>Tasks 1-11b are finished</t>
+  </si>
+  <si>
+    <t>8b</t>
+  </si>
+  <si>
+    <t>Create user stories and add it to doc</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>7  days</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -218,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -232,6 +250,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +547,7 @@
     <col min="5" max="5" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -545,8 +566,11 @@
       <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -565,8 +589,11 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -585,8 +612,11 @@
       <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -605,8 +635,11 @@
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -626,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -646,7 +679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -666,7 +699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -686,7 +719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -706,32 +739,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>25</v>
@@ -740,44 +773,44 @@
         <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>44</v>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>36</v>
@@ -786,55 +819,55 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>47</v>
@@ -848,13 +881,13 @@
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>47</v>
@@ -868,21 +901,41 @@
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Task reviewed and added duration for personas, UXs task
</commit_message>
<xml_diff>
--- a/Tasks/Tasks.xlsx
+++ b/Tasks/Tasks.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>№</t>
   </si>
@@ -181,12 +181,15 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>2 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -536,18 +539,18 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="53.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -570,7 +573,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -593,7 +596,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -616,7 +619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -639,7 +642,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -659,7 +662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -679,7 +682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -698,8 +701,11 @@
       <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -719,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -739,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -759,7 +765,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -779,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -799,7 +805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -819,7 +825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -839,7 +845,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -859,7 +865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -879,7 +885,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -899,7 +905,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -919,7 +925,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added ODATA dev and data generation tasks
</commit_message>
<xml_diff>
--- a/Tasks/Tasks.xlsx
+++ b/Tasks/Tasks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
   <si>
     <t>№</t>
   </si>
@@ -184,12 +184,30 @@
   </si>
   <si>
     <t>2 days</t>
+  </si>
+  <si>
+    <t>ODATA. Add navigation between solution category and solutions</t>
+  </si>
+  <si>
+    <t>ODATA. Implement substringof funtion for solution description field</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>0,5 day</t>
+  </si>
+  <si>
+    <t>Generate test data. Upload data from Historical data xls</t>
+  </si>
+  <si>
+    <t>Task 12 is finished</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -533,21 +551,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="30.26953125" customWidth="1"/>
-    <col min="5" max="5" width="27.7265625" customWidth="1"/>
+    <col min="2" max="2" width="53.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="30.21875" customWidth="1"/>
+    <col min="5" max="5" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -570,7 +588,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -593,7 +611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -616,7 +634,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -639,7 +657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -659,7 +677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -679,7 +697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -702,7 +720,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -725,7 +743,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -748,7 +766,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -768,7 +786,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -788,7 +806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -808,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -828,7 +846,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -848,7 +866,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -868,7 +886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -888,7 +906,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -908,7 +926,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -928,7 +946,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -946,6 +964,75 @@
       </c>
       <c r="F19" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added UI development tasks
</commit_message>
<xml_diff>
--- a/Tasks/Tasks.xlsx
+++ b/Tasks/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
   <si>
     <t>№</t>
   </si>
@@ -202,6 +202,36 @@
   </si>
   <si>
     <t>Task 12 is finished</t>
+  </si>
+  <si>
+    <t>Generate UI (analytics, solutions, solcategoties, tickets)</t>
+  </si>
+  <si>
+    <t>Task 17 is finished</t>
+  </si>
+  <si>
+    <t>Task 16 is finished</t>
+  </si>
+  <si>
+    <t>Task 13 is finished</t>
+  </si>
+  <si>
+    <t>Task 14 is finished</t>
+  </si>
+  <si>
+    <t>Task 15 is finished</t>
+  </si>
+  <si>
+    <t>Start developing Analytics app UI part</t>
+  </si>
+  <si>
+    <t>Start developing Solution Categories app UI part</t>
+  </si>
+  <si>
+    <t>Start developing solutions app UI part</t>
+  </si>
+  <si>
+    <t>Start developing tickets app UI part</t>
   </si>
 </sst>
 </file>
@@ -551,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,6 +1065,97 @@
         <v>52</v>
       </c>
     </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished Odata substring functionality
</commit_message>
<xml_diff>
--- a/Tasks/Tasks.xlsx
+++ b/Tasks/Tasks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="74">
   <si>
     <t>№</t>
   </si>
@@ -594,19 +594,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -629,7 +629,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -652,7 +652,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -675,7 +675,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -698,7 +698,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -718,7 +718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -761,7 +761,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -784,7 +784,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -807,7 +807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -830,7 +830,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -853,7 +853,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -876,7 +876,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -899,7 +899,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -922,7 +922,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -942,7 +942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -965,7 +965,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -985,7 +985,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1103,7 +1103,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1255,11 +1255,14 @@
       <c r="E32" t="s">
         <v>56</v>
       </c>
-      <c r="F32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -1272,8 +1275,11 @@
       <c r="E33" t="s">
         <v>56</v>
       </c>
-      <c r="F33" t="s">
-        <v>38</v>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>